<commit_message>
made new pyco2sys for ctd calcs
</commit_message>
<xml_diff>
--- a/data/flux/rates/RR2018_alk_corrected.xlsx
+++ b/data/flux/rates/RR2018_alk_corrected.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="84">
   <si>
     <t xml:space="preserve">Year</t>
   </si>
@@ -208,6 +208,12 @@
   </si>
   <si>
     <t xml:space="preserve">NO2 Conc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silicate (umol)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phosphate (umol)</t>
   </si>
   <si>
     <t xml:space="preserve">P1 approximate</t>
@@ -456,7 +462,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1668,11 +1674,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="39150304"/>
-        <c:axId val="26691552"/>
+        <c:axId val="94298690"/>
+        <c:axId val="25948079"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="39150304"/>
+        <c:axId val="94298690"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1748,12 +1754,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26691552"/>
+        <c:crossAx val="25948079"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="26691552"/>
+        <c:axId val="25948079"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1829,7 +1835,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39150304"/>
+        <c:crossAx val="94298690"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1891,7 +1897,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3064,11 +3070,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="34582156"/>
-        <c:axId val="17537323"/>
+        <c:axId val="58069308"/>
+        <c:axId val="17011731"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="34582156"/>
+        <c:axId val="58069308"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3144,12 +3150,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17537323"/>
+        <c:crossAx val="17011731"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="17537323"/>
+        <c:axId val="17011731"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3225,7 +3231,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34582156"/>
+        <c:crossAx val="58069308"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12831,10 +12837,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R25"/>
+  <dimension ref="A1:T25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12844,13 +12850,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="27.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="14.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="15.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="10.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="12" style="0" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="14.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="14.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="15.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="10.69"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12884,29 +12891,35 @@
       <c r="J1" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="O1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="P1" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="Q1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="R1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="S1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12941,26 +12954,28 @@
       <c r="J2" s="0" t="n">
         <v>0.914</v>
       </c>
-      <c r="K2" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="L2" s="0" t="s">
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="O2" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="P2" s="0" t="n">
         <f aca="false">H2+0.13</f>
         <v>7.58</v>
       </c>
-      <c r="O2" s="0" t="n">
+      <c r="R2" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="P2" s="0" t="n">
+      <c r="S2" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -12994,26 +13009,28 @@
       <c r="J3" s="0" t="n">
         <v>0.914</v>
       </c>
-      <c r="K3" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="L3" s="0" t="s">
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="O3" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="P3" s="0" t="n">
         <f aca="false">H3+0.13</f>
         <v>7.557</v>
       </c>
-      <c r="O3" s="0" t="n">
+      <c r="R3" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="P3" s="0" t="n">
+      <c r="S3" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="R3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -13047,26 +13064,28 @@
       <c r="J4" s="0" t="n">
         <v>0.914</v>
       </c>
-      <c r="K4" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="L4" s="0" t="s">
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="O4" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="M4" s="0" t="n">
+      <c r="P4" s="0" t="n">
         <f aca="false">H4+0.13</f>
         <v>7.548</v>
       </c>
-      <c r="O4" s="0" t="n">
+      <c r="R4" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="P4" s="0" t="n">
+      <c r="S4" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="T4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="R4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -13100,26 +13119,28 @@
       <c r="J5" s="0" t="n">
         <v>0.908</v>
       </c>
-      <c r="K5" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="L5" s="0" t="s">
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="O5" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="M5" s="0" t="n">
+      <c r="P5" s="0" t="n">
         <f aca="false">H5+0.13</f>
         <v>7.553</v>
       </c>
-      <c r="O5" s="0" t="n">
+      <c r="R5" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="P5" s="0" t="n">
+      <c r="S5" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="R5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -13153,26 +13174,28 @@
       <c r="J6" s="0" t="n">
         <v>0.91</v>
       </c>
-      <c r="K6" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="L6" s="0" t="s">
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="O6" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="M6" s="0" t="n">
+      <c r="P6" s="0" t="n">
         <f aca="false">H6+0.13</f>
         <v>7.548</v>
       </c>
-      <c r="O6" s="0" t="n">
+      <c r="R6" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="P6" s="0" t="n">
+      <c r="S6" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="T6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="R6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -13206,27 +13229,29 @@
       <c r="J7" s="0" t="n">
         <v>0.912</v>
       </c>
-      <c r="K7" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="L7" s="0" t="s">
+      <c r="K7" s="2" t="n">
+        <v>-0.03265926986</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="O7" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="M7" s="0" t="n">
+      <c r="P7" s="0" t="n">
         <f aca="false">H7+0.13</f>
         <v>7.552</v>
       </c>
-      <c r="O7" s="0" t="n">
+      <c r="R7" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="P7" s="0" t="n">
+      <c r="S7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="T7" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="R7" s="2" t="n">
-        <v>-0.03265926986</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13261,27 +13286,29 @@
       <c r="J8" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="L8" s="0" t="s">
+      <c r="K8" s="2" t="n">
+        <v>0.003131710809</v>
+      </c>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="O8" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="M8" s="0" t="n">
+      <c r="P8" s="0" t="n">
         <f aca="false">H8+0.13</f>
         <v>7.557</v>
       </c>
-      <c r="O8" s="0" t="n">
+      <c r="R8" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="P8" s="0" t="n">
+      <c r="S8" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="T8" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="R8" s="2" t="n">
-        <v>0.003131710809</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13316,27 +13343,29 @@
       <c r="J9" s="0" t="n">
         <v>0.906</v>
       </c>
-      <c r="K9" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="L9" s="0" t="s">
+      <c r="K9" s="2" t="n">
+        <v>0.1462956335</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="O9" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="M9" s="0" t="n">
+      <c r="P9" s="0" t="n">
         <f aca="false">H9+0.13</f>
         <v>7.58</v>
       </c>
-      <c r="O9" s="0" t="n">
+      <c r="R9" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="P9" s="0" t="n">
+      <c r="S9" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="T9" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="R9" s="2" t="n">
-        <v>0.1462956335</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13371,27 +13400,29 @@
       <c r="J10" s="0" t="n">
         <v>0.896</v>
       </c>
-      <c r="K10" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="L10" s="0" t="s">
+      <c r="K10" s="2" t="n">
+        <v>0.2178775948</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="O10" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="M10" s="0" t="n">
+      <c r="P10" s="0" t="n">
         <f aca="false">H10+0.13</f>
         <v>7.614</v>
       </c>
-      <c r="O10" s="0" t="n">
+      <c r="R10" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="P10" s="0" t="n">
+      <c r="S10" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="T10" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="R10" s="2" t="n">
-        <v>0.2178775948</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13426,27 +13457,29 @@
       <c r="J11" s="0" t="n">
         <v>0.902</v>
       </c>
-      <c r="K11" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="L11" s="0" t="s">
+      <c r="K11" s="2" t="n">
+        <v>0.2536685755</v>
+      </c>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="O11" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="M11" s="0" t="n">
+      <c r="P11" s="0" t="n">
         <f aca="false">H11+0.13</f>
         <v>7.701</v>
       </c>
-      <c r="O11" s="0" t="n">
+      <c r="R11" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="P11" s="0" t="n">
+      <c r="S11" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="T11" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="R11" s="2" t="n">
-        <v>0.2536685755</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13481,27 +13514,29 @@
       <c r="J12" s="0" t="n">
         <v>0.869</v>
       </c>
-      <c r="K12" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="L12" s="0" t="s">
+      <c r="K12" s="2" t="n">
+        <v>0.3610415175</v>
+      </c>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="O12" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="M12" s="0" t="n">
+      <c r="P12" s="0" t="n">
         <f aca="false">H12+0.13</f>
         <v>7.872</v>
       </c>
-      <c r="O12" s="0" t="n">
+      <c r="R12" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="P12" s="0" t="n">
+      <c r="S12" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="T12" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="R12" s="2" t="n">
-        <v>0.3610415175</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13536,27 +13571,29 @@
       <c r="J13" s="0" t="n">
         <v>0.911</v>
       </c>
-      <c r="K13" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="L13" s="0" t="s">
+      <c r="K13" s="2" t="n">
+        <v>0.2536685755</v>
+      </c>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="O13" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="M13" s="0" t="n">
+      <c r="P13" s="0" t="n">
         <f aca="false">H13+0.13</f>
         <v>8.215</v>
       </c>
-      <c r="O13" s="0" t="n">
+      <c r="R13" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="P13" s="0" t="n">
+      <c r="S13" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="Q13" s="1" t="s">
+      <c r="T13" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="R13" s="2" t="n">
-        <v>0.2536685755</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13591,29 +13628,31 @@
       <c r="J14" s="0" t="n">
         <v>0.918</v>
       </c>
-      <c r="K14" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="L14" s="0" t="s">
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="O14" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="M14" s="0" t="n">
+      <c r="P14" s="0" t="n">
         <f aca="false">H14+0.13</f>
         <v>7.583</v>
       </c>
-      <c r="N14" s="0" t="n">
+      <c r="Q14" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O14" s="0" t="n">
+      <c r="R14" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="P14" s="0" t="n">
+      <c r="S14" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="Q14" s="1" t="n">
+      <c r="T14" s="1" t="n">
         <v>43191.775</v>
       </c>
-      <c r="R14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -13647,30 +13686,32 @@
       <c r="J15" s="0" t="n">
         <v>0.918</v>
       </c>
-      <c r="K15" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="L15" s="0" t="s">
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="O15" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="M15" s="0" t="n">
+      <c r="P15" s="0" t="n">
         <f aca="false">H15+0.13</f>
         <v>7.549</v>
       </c>
-      <c r="N15" s="0" t="n">
+      <c r="Q15" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="O15" s="0" t="n">
+      <c r="R15" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="P15" s="0" t="n">
+      <c r="S15" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="Q15" s="1" t="n">
-        <f aca="false">Q14</f>
+      <c r="T15" s="1" t="n">
+        <f aca="false">T14</f>
         <v>43191.775</v>
       </c>
-      <c r="R15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -13704,30 +13745,32 @@
       <c r="J16" s="0" t="n">
         <v>0.908</v>
       </c>
-      <c r="K16" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="L16" s="0" t="s">
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="O16" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="M16" s="0" t="n">
+      <c r="P16" s="0" t="n">
         <f aca="false">H16+0.13</f>
         <v>7.528</v>
       </c>
-      <c r="N16" s="0" t="n">
+      <c r="Q16" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="O16" s="0" t="n">
+      <c r="R16" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="P16" s="0" t="n">
+      <c r="S16" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="Q16" s="1" t="n">
-        <f aca="false">Q15</f>
+      <c r="T16" s="1" t="n">
+        <f aca="false">T15</f>
         <v>43191.775</v>
       </c>
-      <c r="R16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
@@ -13761,30 +13804,32 @@
       <c r="J17" s="0" t="n">
         <v>0.894</v>
       </c>
-      <c r="K17" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="L17" s="0" t="s">
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="O17" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="M17" s="0" t="n">
+      <c r="P17" s="0" t="n">
         <f aca="false">H17+0.13</f>
         <v>7.544</v>
       </c>
-      <c r="N17" s="0" t="n">
+      <c r="Q17" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="O17" s="0" t="n">
+      <c r="R17" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="P17" s="0" t="n">
+      <c r="S17" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="Q17" s="1" t="n">
-        <f aca="false">Q16</f>
+      <c r="T17" s="1" t="n">
+        <f aca="false">T16</f>
         <v>43191.775</v>
       </c>
-      <c r="R17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
@@ -13818,31 +13863,33 @@
       <c r="J18" s="0" t="n">
         <v>0.915</v>
       </c>
-      <c r="K18" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="L18" s="0" t="s">
+      <c r="K18" s="2" t="n">
+        <v>0.1319558101</v>
+      </c>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="O18" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="M18" s="0" t="n">
+      <c r="P18" s="0" t="n">
         <f aca="false">H18+0.13</f>
         <v>7.566</v>
       </c>
-      <c r="N18" s="0" t="n">
+      <c r="Q18" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="O18" s="0" t="n">
+      <c r="R18" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="P18" s="0" t="n">
+      <c r="S18" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="Q18" s="1" t="n">
-        <f aca="false">Q17</f>
+      <c r="T18" s="1" t="n">
+        <f aca="false">T17</f>
         <v>43191.775</v>
-      </c>
-      <c r="R18" s="2" t="n">
-        <v>0.1319558101</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13877,31 +13924,33 @@
       <c r="J19" s="0" t="n">
         <v>0.908</v>
       </c>
-      <c r="K19" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="L19" s="0" t="s">
+      <c r="K19" s="2" t="n">
+        <v>-0.0521685761</v>
+      </c>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="O19" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="M19" s="0" t="n">
+      <c r="P19" s="0" t="n">
         <f aca="false">H19+0.13</f>
         <v>7.58</v>
       </c>
-      <c r="N19" s="0" t="n">
+      <c r="Q19" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="O19" s="0" t="n">
+      <c r="R19" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="P19" s="0" t="n">
+      <c r="S19" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="Q19" s="1" t="n">
-        <f aca="false">Q18</f>
+      <c r="T19" s="1" t="n">
+        <f aca="false">T18</f>
         <v>43191.775</v>
-      </c>
-      <c r="R19" s="2" t="n">
-        <v>-0.0521685761</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13936,31 +13985,33 @@
       <c r="J20" s="0" t="n">
         <v>0.895</v>
       </c>
-      <c r="K20" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="L20" s="0" t="s">
+      <c r="K20" s="2" t="n">
+        <v>0.6024959083</v>
+      </c>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="O20" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="M20" s="0" t="n">
+      <c r="P20" s="0" t="n">
         <f aca="false">H20+0.13</f>
         <v>7.591</v>
       </c>
-      <c r="N20" s="0" t="n">
+      <c r="Q20" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="O20" s="0" t="n">
+      <c r="R20" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="P20" s="0" t="n">
+      <c r="S20" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="Q20" s="1" t="n">
-        <f aca="false">Q19</f>
+      <c r="T20" s="1" t="n">
+        <f aca="false">T19</f>
         <v>43191.775</v>
-      </c>
-      <c r="R20" s="2" t="n">
-        <v>0.6024959083</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13995,31 +14046,33 @@
       <c r="J21" s="0" t="n">
         <v>0.896</v>
       </c>
-      <c r="K21" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="L21" s="0" t="s">
+      <c r="K21" s="2" t="n">
+        <v>0.3365384615</v>
+      </c>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="O21" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="M21" s="0" t="n">
+      <c r="P21" s="0" t="n">
         <f aca="false">H21+0.13</f>
         <v>7.61</v>
       </c>
-      <c r="N21" s="0" t="n">
+      <c r="Q21" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="O21" s="0" t="n">
+      <c r="R21" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="P21" s="0" t="n">
+      <c r="S21" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="Q21" s="1" t="n">
-        <f aca="false">Q20</f>
+      <c r="T21" s="1" t="n">
+        <f aca="false">T20</f>
         <v>43191.775</v>
-      </c>
-      <c r="R21" s="2" t="n">
-        <v>0.3365384615</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14054,31 +14107,33 @@
       <c r="J22" s="0" t="n">
         <v>0.896</v>
       </c>
-      <c r="K22" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="L22" s="0" t="s">
+      <c r="K22" s="2" t="n">
+        <v>0.09103927987</v>
+      </c>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="O22" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="M22" s="0" t="n">
+      <c r="P22" s="0" t="n">
         <f aca="false">H22+0.13</f>
         <v>7.722</v>
       </c>
-      <c r="N22" s="0" t="n">
+      <c r="Q22" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="O22" s="0" t="n">
+      <c r="R22" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="P22" s="0" t="n">
+      <c r="S22" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="Q22" s="1" t="n">
-        <f aca="false">Q21</f>
+      <c r="T22" s="1" t="n">
+        <f aca="false">T21</f>
         <v>43191.775</v>
-      </c>
-      <c r="R22" s="2" t="n">
-        <v>0.09103927987</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14113,31 +14168,33 @@
       <c r="J23" s="0" t="n">
         <v>0.896</v>
       </c>
-      <c r="K23" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="L23" s="0" t="s">
+      <c r="K23" s="2" t="n">
+        <v>-0.3385842881</v>
+      </c>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="O23" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="M23" s="0" t="n">
+      <c r="P23" s="0" t="n">
         <f aca="false">H23+0.13</f>
         <v>7.696</v>
       </c>
-      <c r="N23" s="0" t="n">
+      <c r="Q23" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="O23" s="0" t="n">
+      <c r="R23" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="P23" s="0" t="n">
+      <c r="S23" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="Q23" s="1" t="n">
-        <f aca="false">Q22</f>
+      <c r="T23" s="1" t="n">
+        <f aca="false">T22</f>
         <v>43191.775</v>
-      </c>
-      <c r="R23" s="2" t="n">
-        <v>-0.3385842881</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14172,31 +14229,33 @@
       <c r="J24" s="0" t="n">
         <v>0.898</v>
       </c>
-      <c r="K24" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="L24" s="0" t="s">
+      <c r="K24" s="2" t="n">
+        <v>-0.2158346972</v>
+      </c>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="O24" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="M24" s="0" t="n">
+      <c r="P24" s="0" t="n">
         <f aca="false">H24+0.13</f>
         <v>8.2</v>
       </c>
-      <c r="N24" s="0" t="n">
+      <c r="Q24" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="O24" s="0" t="n">
+      <c r="R24" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="P24" s="0" t="n">
+      <c r="S24" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="Q24" s="1" t="n">
-        <f aca="false">Q23</f>
+      <c r="T24" s="1" t="n">
+        <f aca="false">T23</f>
         <v>43191.775</v>
-      </c>
-      <c r="R24" s="2" t="n">
-        <v>-0.2158346972</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14231,31 +14290,33 @@
       <c r="J25" s="0" t="n">
         <v>0.9</v>
       </c>
-      <c r="K25" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="L25" s="0" t="s">
+      <c r="K25" s="2" t="n">
+        <v>-0.481792144</v>
+      </c>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="O25" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="M25" s="0" t="n">
+      <c r="P25" s="0" t="n">
         <f aca="false">H25+0.13</f>
         <v>8.248</v>
       </c>
-      <c r="N25" s="0" t="n">
+      <c r="Q25" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="O25" s="0" t="n">
+      <c r="R25" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="P25" s="0" t="n">
+      <c r="S25" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="Q25" s="1" t="n">
-        <f aca="false">Q24</f>
+      <c r="T25" s="1" t="n">
+        <f aca="false">T24</f>
         <v>43191.775</v>
-      </c>
-      <c r="R25" s="2" t="n">
-        <v>-0.481792144</v>
       </c>
     </row>
   </sheetData>
@@ -14284,67 +14345,67 @@
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="T1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="V1" s="2" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
finished p2 ctd dic calc nb
</commit_message>
<xml_diff>
--- a/data/flux/rates/RR2018_alk_corrected.xlsx
+++ b/data/flux/rates/RR2018_alk_corrected.xlsx
@@ -515,7 +515,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1727,11 +1727,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="63099385"/>
-        <c:axId val="12594884"/>
+        <c:axId val="75012274"/>
+        <c:axId val="4996157"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63099385"/>
+        <c:axId val="75012274"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1807,12 +1807,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12594884"/>
+        <c:crossAx val="4996157"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="12594884"/>
+        <c:axId val="4996157"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1888,7 +1888,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63099385"/>
+        <c:crossAx val="75012274"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1950,7 +1950,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3123,11 +3123,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="21636354"/>
-        <c:axId val="78211070"/>
+        <c:axId val="11966736"/>
+        <c:axId val="18488236"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="21636354"/>
+        <c:axId val="11966736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3203,12 +3203,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78211070"/>
+        <c:crossAx val="18488236"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="78211070"/>
+        <c:axId val="18488236"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3284,7 +3284,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21636354"/>
+        <c:crossAx val="11966736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -17126,8 +17126,8 @@
   </sheetPr>
   <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M16" activeCellId="0" sqref="M16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M26" activeCellId="0" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18075,6 +18075,9 @@
       <c r="L16" s="0" t="n">
         <v>3.34</v>
       </c>
+      <c r="M16" s="0" t="n">
+        <v>2.53</v>
+      </c>
       <c r="N16" s="0" t="n">
         <v>0.908</v>
       </c>
@@ -18133,6 +18136,9 @@
       <c r="L17" s="0" t="n">
         <v>3.23</v>
       </c>
+      <c r="M17" s="0" t="n">
+        <v>2.48</v>
+      </c>
       <c r="N17" s="0" t="n">
         <v>0.894</v>
       </c>
@@ -18191,6 +18197,9 @@
       <c r="L18" s="0" t="n">
         <v>2.92</v>
       </c>
+      <c r="M18" s="0" t="n">
+        <v>2.52</v>
+      </c>
       <c r="N18" s="0" t="n">
         <v>0.915</v>
       </c>
@@ -18251,6 +18260,9 @@
       <c r="L19" s="0" t="n">
         <v>2.75</v>
       </c>
+      <c r="M19" s="0" t="n">
+        <v>2.49</v>
+      </c>
       <c r="N19" s="0" t="n">
         <v>0.908</v>
       </c>
@@ -18311,6 +18323,9 @@
       <c r="L20" s="0" t="n">
         <v>2.69</v>
       </c>
+      <c r="M20" s="0" t="n">
+        <v>2.45</v>
+      </c>
       <c r="N20" s="0" t="n">
         <v>0.895</v>
       </c>
@@ -18371,6 +18386,9 @@
       <c r="L21" s="0" t="n">
         <v>2.61</v>
       </c>
+      <c r="M21" s="0" t="n">
+        <v>2.44</v>
+      </c>
       <c r="N21" s="0" t="n">
         <v>0.896</v>
       </c>
@@ -18431,6 +18449,9 @@
       <c r="L22" s="0" t="n">
         <v>2.43</v>
       </c>
+      <c r="M22" s="0" t="n">
+        <v>2.39</v>
+      </c>
       <c r="N22" s="0" t="n">
         <v>0.896</v>
       </c>
@@ -18491,6 +18512,9 @@
       <c r="L23" s="0" t="n">
         <v>2.27</v>
       </c>
+      <c r="M23" s="0" t="n">
+        <v>2.4</v>
+      </c>
       <c r="N23" s="0" t="n">
         <v>0.896</v>
       </c>
@@ -18551,6 +18575,9 @@
       <c r="L24" s="0" t="n">
         <v>0.28</v>
       </c>
+      <c r="M24" s="0" t="n">
+        <v>2.07</v>
+      </c>
       <c r="N24" s="0" t="n">
         <v>0.898</v>
       </c>
@@ -18610,6 +18637,9 @@
       </c>
       <c r="L25" s="0" t="n">
         <v>0.21</v>
+      </c>
+      <c r="M25" s="0" t="n">
+        <v>2.02</v>
       </c>
       <c r="N25" s="0" t="n">
         <v>0.9</v>

</xml_diff>